<commit_message>
Commit after adding all the responces from the API to the lur page.
</commit_message>
<xml_diff>
--- a/Resources/oxfordAPIDM.xlsx
+++ b/Resources/oxfordAPIDM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zuac-my.sharepoint.com/personal/m80007966_zu_ac_ae/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siem Ghirmai\Documents\Projects\Dictionary\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E4C7C8-525B-4406-98CD-87B06700EAB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="31">
   <si>
     <t>DICTIONARY</t>
   </si>
@@ -114,12 +115,18 @@
   </si>
   <si>
     <t>result structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'id': 'firebug', 'metadata': {'operation': 'retrieve', 'provider': 'Oxford University Press', 'schema': 'RetrieveEntry'}, 'results': [{'id': 'firebug', 'language': 'en-gb', 'lexicalEntries': [{'entries': [{'senses': [{'definitions': ['an arsonist.'], 'id': 'm_en_gbus0364130.005'}]}], 'language': 'en-gb', 'lexicalCategory': {'id': 'noun', 'text': 'Noun'}, 'text': 'firebug'}], 'type': 'headword', </t>
+  </si>
+  <si>
+    <t>'word': 'firebug'}], 'word': 'firebug'}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -223,6 +230,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -490,23 +500,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V57"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A33" zoomScale="85" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" customWidth="1"/>
-    <col min="6" max="6" width="29.1640625" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.875" customWidth="1"/>
+    <col min="5" max="5" width="17.125" customWidth="1"/>
+    <col min="6" max="6" width="29.125" customWidth="1"/>
+    <col min="10" max="10" width="19.625" customWidth="1"/>
+    <col min="12" max="12" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J2" t="s">
         <v>1</v>
       </c>
@@ -549,22 +559,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I6" t="s">
         <v>4</v>
       </c>
@@ -572,12 +582,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>4</v>
       </c>
@@ -597,17 +607,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>28</v>
       </c>
@@ -633,17 +643,17 @@
       <c r="U17" s="12"/>
       <c r="V17" s="12"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -654,12 +664,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>10</v>
       </c>
@@ -682,27 +692,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J23" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J24" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J25" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I27" t="s">
         <v>16</v>
       </c>
@@ -716,7 +726,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J28" s="3"/>
       <c r="K28" t="s">
         <v>15</v>
@@ -724,7 +734,7 @@
       <c r="L28" s="8"/>
       <c r="M28" s="7"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J29" s="3" t="s">
         <v>20</v>
       </c>
@@ -736,7 +746,7 @@
       </c>
       <c r="M29" s="7"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J30" s="3"/>
       <c r="K30" t="s">
         <v>15</v>
@@ -744,7 +754,7 @@
       <c r="L30" s="8"/>
       <c r="M30" s="7"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J31" s="3" t="s">
         <v>21</v>
       </c>
@@ -756,7 +766,7 @@
       </c>
       <c r="M31" s="7"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J32" s="4"/>
       <c r="K32" t="s">
         <v>15</v>
@@ -764,7 +774,7 @@
       <c r="L32" s="8"/>
       <c r="M32" s="7"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
         <v>20</v>
       </c>
@@ -775,17 +785,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="I34" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
         <v>22</v>
       </c>
@@ -793,12 +803,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>20</v>
       </c>
@@ -818,17 +828,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="I39" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
         <v>25</v>
       </c>
@@ -836,22 +846,22 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>20</v>
       </c>
@@ -859,12 +869,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>10</v>
       </c>
@@ -890,17 +900,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="I48" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
         <v>25</v>
       </c>
@@ -908,19 +918,29 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E51" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>